<commit_message>
feat: comprehensive dashboard and alerts enhancements
- Enhanced alerts panel with filtering and sorting capabilities
- Fixed dashboard layout with proper height constraints
- Improved map display and scrolling functionality
- Added alert simulation for testing
- Better container-wise alert organization
- Enhanced UI components and responsive design
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-24.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-24.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="35">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,19 +43,79 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-24T06:49:35.073Z</t>
+    <t>2025-11-24T09:31:23.964Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1e5a6344-83d3-48e9-bc1a-0dfcb0be8813","EventDtm":"2025-11-24T06:44:52Z","AppDtm":"2025-11-24T06:45:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T06:44:52Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":17.533176,"GPSLongitude":78.433601,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":47,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T06:44:52Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":29.69,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":80,"TDisQ":null,"FreqComp":null,"TSuc":-28.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":890,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":410.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.12,"TRtn1Q":null,"TRtn2":6.1,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.37,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T06:49:35.111Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"32ca944e-7c8f-4bfb-9516-728cd183fe8c","EventDtm":"2025-11-24T06:48:58Z","AppDtm":"2025-11-24T06:49:13Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T06:48:58Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.657975,"GPSLongitude":83.101798,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8.1,"DeviceTemp":39,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T06:48:58Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":34.07,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":70.1,"PSucQ":null,"TDis":-191.02,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":131.36,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.92,"AmpPhB":1.55,"AmpPhC":0.92,"PDis":131.57,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.91,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":420.85,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.69,"TRtn1Q":null,"TRtn2":20.75,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":15.05,"PctSucVlvQ":null,"TSup1":20.12,"TSup1Q":null,"TSup2":20.2,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d675a633-726c-4afd-b83e-b772176abf33","EventDtm":"2025-11-24T09:31:03Z","AppDtm":"2025-11-24T09:31:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:31:03Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657838,"GPSLongitude":83.101784,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"248666913","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":7.9,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:31:03Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":29.85,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":65.86,"PSucQ":null,"TDis":-191.8,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":137.31,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.92,"AmpPhB":1.54,"AmpPhC":0.92,"PDis":150.14,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.4,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.26,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.09,"TRtn1Q":null,"TRtn2":20.1,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":18.49,"PctSucVlvQ":null,"TSup1":18.99,"TSup1Q":null,"TSup2":19.07,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:31:36.082Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"92c925a0-c632-4961-ba83-f560fef5c6e6","EventDtm":"2025-11-24T09:31:20Z","AppDtm":"2025-11-24T09:31:34Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:31:20Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.572157,"GPSLongitude":78.514977,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323414","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:31:41.777Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"96ac87a5-715d-4072-91ee-515eb562ea66","EventDtm":"2025-11-24T09:31:24Z","AppDtm":"2025-11-24T09:31:41Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:31:24Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.805008,"GPSLongitude":77.662269,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:31:24Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":28.98,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":168.39,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.08,"AmpPhB":10.52,"AmpPhC":10.08,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.02,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.42,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.49,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.05,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.48,"TRtn1Q":null,"TRtn2":5.48,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":3.17,"PctSucVlvQ":null,"TSup1":4.96,"TSup1Q":null,"TSup2":4.98,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:32:42.721Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"991ea4d3-36a7-491a-996d-3ecdf304092d","EventDtm":"2025-11-24T09:32:26Z","AppDtm":"2025-11-24T09:32:42Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:32:26Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":26.606171,"GPSLongitude":80.723755,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":false,"ExtPowerVoltage":6,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:33:15.758Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6f9d257f-37a2-4637-bfef-217051800198","EventDtm":"2025-11-24T09:33:01Z","AppDtm":"2025-11-24T09:33:15Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:33:01Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":12.805058,"GPSLongitude":77.662234,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:33:01Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.34,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":106.15,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.32,"AmpPhB":10.61,"AmpPhC":11.32,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.26,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.82,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.1,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.82,"TRtn1Q":null,"TRtn2":5.84,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.37,"PctSucVlvQ":null,"TSup1":5.11,"TSup1Q":null,"TSup2":5.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:33:51.779Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"17dfc11f-308c-4efd-8d45-00a9ec77313b","EventDtm":"2025-11-24T09:33:34Z","AppDtm":"2025-11-24T09:33:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:33:34Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.679088,"GPSLongitude":78.720172,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":44,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:33:34Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":29.86,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-181.25,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":155.96,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.29,"AmpPhB":10.92,"AmpPhC":11.29,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.46,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":98.81,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.67,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.11,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.02,"TRtn1Q":null,"TRtn2":5.01,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.45,"PctSucVlvQ":null,"TSup1":3.89,"TSup1Q":null,"TSup2":3.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:35:52.733Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0a8ac7fd-78ad-4734-b2b5-ba149232e16d","EventDtm":"2025-11-24T09:35:38Z","AppDtm":"2025-11-24T09:35:52Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:35:38Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":26.310566,"GPSLongitude":91.717636,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551307","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.2,"BatteryVoltage":8.1,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:35:38Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":28.81,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":73.3,"TDisQ":null,"FreqComp":null,"TSuc":-25.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":960,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":72,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":393.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":92.07,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:43:13.486Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"49130eb5-9e5c-4536-928f-5c3b18928cfa","EventDtm":"2025-11-24T09:42:59Z","AppDtm":"2025-11-24T09:43:13Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:42:59Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.80506,"GPSLongitude":77.662245,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:42:59Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.86,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":103.09,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.25,"AmpPhB":10.79,"AmpPhC":11.25,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.25,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.76,"TRtn1Q":null,"TRtn2":5.78,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.84,"PctSucVlvQ":null,"TSup1":4.94,"TSup1Q":null,"TSup2":4.86,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:45:45.274Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4e06f62b-61d0-4b73-a9ef-a1c6df014d68","EventDtm":"2025-11-24T09:45:28Z","AppDtm":"2025-11-24T09:45:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:45:28Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.53317,"GPSLongitude":78.433499,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":44,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:45:28Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":31.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":78,"TDisQ":null,"FreqComp":null,"TSuc":-27.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":940,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":410.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.31,"TRtn1Q":null,"TRtn2":6.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.28,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:48:38.612Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"54ea56e8-0ba0-479f-b956-c087919f815f","EventDtm":"2025-11-24T09:48:24Z","AppDtm":"2025-11-24T09:48:38Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:48:24Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":17.657914,"GPSLongitude":83.101831,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":28.6,"BatteryVoltage":8.1,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:48:24Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":29.49,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":16.22,"PSucQ":null,"TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":226.04,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04783085","AmpPhA":17.41,"AmpPhB":17.77,"AmpPhC":17.41,"PDis":240.44,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.14,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":399.02,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.69,"TRtn1Q":null,"TRtn2":20.74,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":22.02,"PctSucVlvQ":null,"TSup1":17.96,"TSup1Q":null,"TSup2":18.02,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:50:25.399Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5f7c45c9-f84d-4b13-a9ed-14334ddd0e7e","EventDtm":"2025-11-24T09:50:06Z","AppDtm":"2025-11-24T09:50:24Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:50:06Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":28.678773,"GPSLongitude":77.59983,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.1,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:50:06Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":24.19,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":70.74,"PSucQ":null,"TDis":33.09,"TDisQ":null,"FreqComp":null,"TSuc":20.87,"TSucQ":null,"MCond":0,"PCond":306.05,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04475864","AmpPhA":1.58,"AmpPhB":1.56,"AmpPhC":1.58,"PDis":84.31,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.14,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":61.62,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":409.54,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":21.69,"TRtn1Q":null,"TRtn2":21.67,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":10,"PctSucVlvQ":null,"TSup1":20.51,"TSup1Q":null,"TSup2":20.41,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T09:51:17.401Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5f4b9f47-d565-42ee-9865-0558679c5965","EventDtm":"2025-11-24T09:48:34Z","AppDtm":"2025-11-24T09:51:17Z","Events":["DeviceIsStationary"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:48:34Z","DeviceID":"JSGA622180064","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.829046,"GPSLongitude":76.793505,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"864","LAC":"91","CID":"6906161","RSSI":null,"ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.4,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1041571","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
   </si>
 </sst>
 </file>
@@ -444,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -559,6 +619,326 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
no changes Client flow updates for 25 Nov
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-24.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-24.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="121">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,79 +43,337 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-24T09:31:23.964Z</t>
+    <t>2025-11-24T12:12:33.706Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d675a633-726c-4afd-b83e-b772176abf33","EventDtm":"2025-11-24T09:31:03Z","AppDtm":"2025-11-24T09:31:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:31:03Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657838,"GPSLongitude":83.101784,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"248666913","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":7.9,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:31:03Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":29.85,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":65.86,"PSucQ":null,"TDis":-191.8,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":137.31,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.92,"AmpPhB":1.54,"AmpPhC":0.92,"PDis":150.14,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.4,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.26,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.09,"TRtn1Q":null,"TRtn2":20.1,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":18.49,"PctSucVlvQ":null,"TSup1":18.99,"TSup1Q":null,"TSup2":19.07,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:31:36.082Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"92c925a0-c632-4961-ba83-f560fef5c6e6","EventDtm":"2025-11-24T09:31:20Z","AppDtm":"2025-11-24T09:31:34Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:31:20Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.572157,"GPSLongitude":78.514977,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323414","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:31:41.777Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"96ac87a5-715d-4072-91ee-515eb562ea66","EventDtm":"2025-11-24T09:31:24Z","AppDtm":"2025-11-24T09:31:41Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:31:24Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.805008,"GPSLongitude":77.662269,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:31:24Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":28.98,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":168.39,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.08,"AmpPhB":10.52,"AmpPhC":10.08,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.02,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.42,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.49,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.05,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.48,"TRtn1Q":null,"TRtn2":5.48,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":3.17,"PctSucVlvQ":null,"TSup1":4.96,"TSup1Q":null,"TSup2":4.98,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:32:42.721Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"991ea4d3-36a7-491a-996d-3ecdf304092d","EventDtm":"2025-11-24T09:32:26Z","AppDtm":"2025-11-24T09:32:42Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:32:26Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":26.606171,"GPSLongitude":80.723755,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":false,"ExtPowerVoltage":6,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:33:15.758Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6f9d257f-37a2-4637-bfef-217051800198","EventDtm":"2025-11-24T09:33:01Z","AppDtm":"2025-11-24T09:33:15Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:33:01Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":12.805058,"GPSLongitude":77.662234,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:33:01Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.34,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":106.15,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.32,"AmpPhB":10.61,"AmpPhC":11.32,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.26,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.82,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.1,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.82,"TRtn1Q":null,"TRtn2":5.84,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.37,"PctSucVlvQ":null,"TSup1":5.11,"TSup1Q":null,"TSup2":5.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:33:51.779Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"17dfc11f-308c-4efd-8d45-00a9ec77313b","EventDtm":"2025-11-24T09:33:34Z","AppDtm":"2025-11-24T09:33:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:33:34Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.679088,"GPSLongitude":78.720172,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":44,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:33:34Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":29.86,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-181.25,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":155.96,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.29,"AmpPhB":10.92,"AmpPhC":11.29,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.46,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":98.81,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.67,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.11,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.02,"TRtn1Q":null,"TRtn2":5.01,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.45,"PctSucVlvQ":null,"TSup1":3.89,"TSup1Q":null,"TSup2":3.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:35:52.733Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0a8ac7fd-78ad-4734-b2b5-ba149232e16d","EventDtm":"2025-11-24T09:35:38Z","AppDtm":"2025-11-24T09:35:52Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:35:38Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":26.310566,"GPSLongitude":91.717636,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551307","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.2,"BatteryVoltage":8.1,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:35:38Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":28.81,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":73.3,"TDisQ":null,"FreqComp":null,"TSuc":-25.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":960,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":72,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":393.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":92.07,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:43:13.486Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"49130eb5-9e5c-4536-928f-5c3b18928cfa","EventDtm":"2025-11-24T09:42:59Z","AppDtm":"2025-11-24T09:43:13Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:42:59Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.80506,"GPSLongitude":77.662245,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:42:59Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.86,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":103.09,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.25,"AmpPhB":10.79,"AmpPhC":11.25,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.25,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.76,"TRtn1Q":null,"TRtn2":5.78,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.84,"PctSucVlvQ":null,"TSup1":4.94,"TSup1Q":null,"TSup2":4.86,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:45:45.274Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4e06f62b-61d0-4b73-a9ef-a1c6df014d68","EventDtm":"2025-11-24T09:45:28Z","AppDtm":"2025-11-24T09:45:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:45:28Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.53317,"GPSLongitude":78.433499,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":44,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:45:28Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":31.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":78,"TDisQ":null,"FreqComp":null,"TSuc":-27.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":940,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":410.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.31,"TRtn1Q":null,"TRtn2":6.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.28,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:48:38.612Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"54ea56e8-0ba0-479f-b956-c087919f815f","EventDtm":"2025-11-24T09:48:24Z","AppDtm":"2025-11-24T09:48:38Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:48:24Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":17.657914,"GPSLongitude":83.101831,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":28.6,"BatteryVoltage":8.1,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:48:24Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":29.49,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":16.22,"PSucQ":null,"TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":226.04,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04783085","AmpPhA":17.41,"AmpPhB":17.77,"AmpPhC":17.41,"PDis":240.44,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.14,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":399.02,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.69,"TRtn1Q":null,"TRtn2":20.74,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":22.02,"PctSucVlvQ":null,"TSup1":17.96,"TSup1Q":null,"TSup2":18.02,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:50:25.399Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5f7c45c9-f84d-4b13-a9ed-14334ddd0e7e","EventDtm":"2025-11-24T09:50:06Z","AppDtm":"2025-11-24T09:50:24Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:50:06Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":28.678773,"GPSLongitude":77.59983,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.1,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T09:50:06Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":24.19,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":70.74,"PSucQ":null,"TDis":33.09,"TDisQ":null,"FreqComp":null,"TSuc":20.87,"TSucQ":null,"MCond":0,"PCond":306.05,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04475864","AmpPhA":1.58,"AmpPhB":1.56,"AmpPhC":1.58,"PDis":84.31,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.14,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":61.62,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":409.54,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":21.69,"TRtn1Q":null,"TRtn2":21.67,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":10,"PctSucVlvQ":null,"TSup1":20.51,"TSup1Q":null,"TSup2":20.41,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-24T09:51:17.401Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5f4b9f47-d565-42ee-9865-0558679c5965","EventDtm":"2025-11-24T09:48:34Z","AppDtm":"2025-11-24T09:51:17Z","Events":["DeviceIsStationary"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T09:48:34Z","DeviceID":"JSGA622180064","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.829046,"GPSLongitude":76.793505,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"864","LAC":"91","CID":"6906161","RSSI":null,"ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.4,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1041571","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c9da9e39-7c52-4c85-91cc-913a8336dce3","EventDtm":"2025-11-24T10:33:42Z","AppDtm":"2025-11-24T10:33:59Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:33:42Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.679072,"GPSLongitude":78.720173,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:33:42Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":28.99,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.03,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":152.04,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.22,"AmpPhB":10.7,"AmpPhC":11.22,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.44,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":98.45,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":408.99,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.97,"TRtn1Q":null,"TRtn2":4.97,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.04,"PctSucVlvQ":null,"TSup1":3.96,"TSup1Q":null,"TSup2":3.99,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.781Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"46cf514b-f7d2-4a47-8ac5-ae52081eaab3","EventDtm":"2025-11-24T10:34:45Z","AppDtm":"2025-11-24T10:35:01Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:34:45Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.678757,"GPSLongitude":78.720205,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.1,"BatteryVoltage":8.1,"DeviceTemp":44,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:34:45Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":32,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":320,"PSucQ":"asProvided","TDis":36.8,"TDisQ":null,"FreqComp":null,"TSuc":38.1,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":710,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":400,"PctExpVlvQ":"OOR","TEvap":11.31,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":66.93,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":398.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":13.19,"TRtn1Q":null,"TRtn2":12.9,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":14.12,"TSup1Q":null,"TSup2":14.1,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.874Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"aab89695-2fea-41f1-85c3-2cc793386029","EventDtm":"2025-11-24T10:35:43Z","AppDtm":"2025-11-24T10:35:58Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:35:43Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":26.310578,"GPSLongitude":91.717614,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551307","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.1,"BatteryVoltage":8.1,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:35:43Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":25.81,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":71.5,"TDisQ":null,"FreqComp":null,"TSuc":-24.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":880,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":72,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":391.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":87.5,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":3.7,"TSup2Q":null,"AmpTotalDraw":10,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.886Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ae360521-29fc-4605-ac64-c67e9a5791b3","EventDtm":"2025-11-24T10:42:59Z","AppDtm":"2025-11-24T10:43:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:42:59Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.805074,"GPSLongitude":77.662274,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:42:59Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.37,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":102.24,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.88,"AmpPhB":11.27,"AmpPhC":11.88,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.2,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.21,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.76,"TRtn1Q":null,"TRtn2":5.78,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.12,"PctSucVlvQ":null,"TSup1":4.94,"TSup1Q":null,"TSup2":4.87,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.895Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e3831e83-bc6d-4186-9a2e-6bca9706262c","EventDtm":"2025-11-24T10:45:36Z","AppDtm":"2025-11-24T10:45:54Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:45:36Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.533248,"GPSLongitude":78.433449,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:45:36Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":30,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":75.9,"TDisQ":null,"FreqComp":null,"TSuc":-28.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":410.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.31,"TRtn1Q":null,"TRtn2":6.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.915Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1755fc83-5360-4ba0-9d4a-37110a30e1e6","EventDtm":"2025-11-24T10:48:15Z","AppDtm":"2025-11-24T10:48:29Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:48:15Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657936,"GPSLongitude":83.10179,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:48:15Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":29.49,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":70.37,"PSucQ":null,"TDis":-191.02,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":115.29,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.92,"AmpPhB":1.55,"AmpPhC":0.92,"PDis":115.29,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.92,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.03,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":421.07,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.63,"TRtn1Q":null,"TRtn2":20.69,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":18.8,"PctSucVlvQ":null,"TSup1":20.35,"TSup1Q":null,"TSup2":20.43,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.932Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fb3898da-cdf3-4c5e-a0af-cfe1814b2dbc","EventDtm":"2025-11-24T10:49:41Z","AppDtm":"2025-11-24T10:50:01Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:49:41Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":28.678788,"GPSLongitude":77.599733,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230078045","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:49:41Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":24.79,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":61.77,"PSucQ":null,"TDis":61.8,"TDisQ":null,"FreqComp":null,"TSuc":17.62,"TSucQ":null,"MCond":0,"PCond":274.28,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04475864","AmpPhA":1.58,"AmpPhB":1.54,"AmpPhC":1.58,"PDis":107.29,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":17.79,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":70.94,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":403.33,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.32,"TRtn1Q":null,"TRtn2":17.32,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":20,"PctSucVlvQ":null,"TSup1":17.92,"TSup1Q":null,"TSup2":17.95,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.941Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d503d854-5127-447e-8704-355a29265363","EventDtm":"2025-11-24T10:53:00Z","AppDtm":"2025-11-24T10:53:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:53:00Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.805054,"GPSLongitude":77.662174,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:53:00Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.12,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":100.89,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.69,"AmpPhB":10.98,"AmpPhC":11.69,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.16,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.54,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.02,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.72,"TRtn1Q":null,"TRtn2":5.74,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.66,"PctSucVlvQ":null,"TSup1":4.98,"TSup1Q":null,"TSup2":4.92,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.964Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"aa6dd074-a119-4e4e-b1fa-831dfcc08413","EventDtm":"2025-11-24T10:53:23Z","AppDtm":"2025-11-24T10:53:38Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:53:23Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":17.539002,"GPSLongitude":78.17825,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:53:23Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":30.12,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":112.7,"TDisQ":null,"FreqComp":null,"TSuc":-32.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":980,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":3.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":402.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.12,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":93.9,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.974Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1c8972fc-68f6-4e2a-8d20-0dbd6c29d422","EventDtm":"2025-11-24T10:59:25Z","AppDtm":"2025-11-24T10:59:40Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:59:25Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":26.644592,"GPSLongitude":88.468017,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:59:25Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":25.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":60.3,"TDisQ":null,"FreqComp":null,"TSuc":-25.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":890,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":36,"PctExpVlvQ":null,"TEvap":-0.88,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":406.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":0.69,"TRtn1Q":null,"TRtn2":1.5,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.89,"PctSucVlvQ":null,"TSup1":0,"TSup1Q":null,"TSup2":1.7,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.978Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f33e0eb3-3025-48e7-9420-a52ded66db9b","EventDtm":"2025-11-24T10:59:49Z","AppDtm":"2025-11-24T11:00:08Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T10:59:49Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.824875,"GPSLongitude":78.131515,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T10:59:49Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":31.69,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":10,"PSucQ":"asProvided","TDis":75.3,"TDisQ":null,"FreqComp":null,"TSuc":-23.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1130,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":11.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":390.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.38,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.59,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":16,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.991Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6f6fa0b8-d4d0-4190-ab77-1fb6d85a6e64","EventDtm":"2025-11-24T11:01:26Z","AppDtm":"2025-11-24T11:01:43Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:01:26Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":21.735695,"GPSLongitude":72.628909,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31.3,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:01:26Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":33.24,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":187.97,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":13.52,"AmpPhB":13.34,"AmpPhC":13.52,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.38,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":89,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":434.41,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.07,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.66,"TRtn1Q":null,"TRtn2":15.61,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":2.29,"PctSucVlvQ":null,"TSup1":15.06,"TSup1Q":null,"TSup2":15.25,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:33.995Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9cffec08-639f-415c-8502-29b70af62e6e","EventDtm":"2025-11-24T11:01:35Z","AppDtm":"2025-11-24T11:01:50Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:01:35Z","DeviceID":"JSGA623040329","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":1,"GPSLatitude":17.548083,"GPSLongitude":78.380666,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-53","ExtPower":true,"ExtPowerVoltage":33.2,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.000Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9cedb793-78c8-4aba-ab96-237ca25abc82","EventDtm":"2025-11-24T11:03:05Z","AppDtm":"2025-11-24T11:03:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:03:05Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.805029,"GPSLongitude":77.662134,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:03:05Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.2,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":100.97,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.77,"AmpPhB":10.92,"AmpPhC":11.77,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.27,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.06,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.77,"TRtn1Q":null,"TRtn2":5.79,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.32,"PctSucVlvQ":null,"TSup1":5.06,"TSup1Q":null,"TSup2":4.98,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.011Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"86765d9b-9e73-4273-8fb2-aed0e1f7d617","EventDtm":"2025-11-24T11:04:39Z","AppDtm":"2025-11-24T11:04:54Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:04:39Z","DeviceID":"JSGA623040302","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":18,"GPSLatitude":19.252882,"GPSLongitude":73.016427,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":28.7,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.019Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a3d79115-3464-44cb-ac0b-f16e57151184","EventDtm":"2025-11-24T12:51:19Z","AppDtm":"2025-11-24T11:10:01Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T12:51:19Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":2620,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":33.9,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.026Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"706e57fa-c691-4276-a9d0-a1674d59f40a","EventDtm":"2025-11-24T11:11:04Z","AppDtm":"2025-11-24T11:11:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:11:04Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":17.661614,"GPSLongitude":83.089141,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.2,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:11:04Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":30.88,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":46.5,"TDisQ":null,"FreqComp":null,"TSuc":-13.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1070,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":360.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.38,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":99.39,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.7,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.027Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"13718bb5-7654-4685-8017-54e57790e84e","EventDtm":"2025-11-24T11:11:16Z","AppDtm":"2025-11-24T11:11:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:11:16Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.572298,"GPSLongitude":78.515002,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323414","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.037Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"01b04b1f-32ae-4a0f-9035-df50accb9584","EventDtm":"2025-11-24T11:13:01Z","AppDtm":"2025-11-24T11:13:15Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:13:01Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.80502,"GPSLongitude":77.662159,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:13:01Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.94,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":100.15,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.64,"AmpPhB":11.24,"AmpPhC":11.64,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.17,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.78,"TRtn1Q":null,"TRtn2":5.81,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.35,"PctSucVlvQ":null,"TSup1":4.99,"TSup1Q":null,"TSup2":4.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.041Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"27623684-9964-443b-9383-74e2649fd8c2","EventDtm":"2025-11-24T11:13:23Z","AppDtm":"2025-11-24T11:13:39Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:13:23Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.537153,"GPSLongitude":78.175637,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":27.4,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:13:23Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":28.31,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":116.41,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":9.82,"AmpPhB":10.18,"AmpPhC":9.82,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-25.65,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":19.26,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":386.31,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.44,"TRtn1Q":null,"TRtn2":-17.45,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.3,"TSup1Q":null,"TSup2":-31.21,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.086Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fbeb0fcf-60ec-4fc9-9cd2-c72e3fb981af","EventDtm":"2025-11-24T11:14:14Z","AppDtm":"2025-11-24T11:14:29Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:14:14Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.547795,"GPSLongitude":78.380491,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.2,"BatteryVoltage":8.1,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.087Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"875f73cf-efe9-4c16-9de7-078d7242e9b2","EventDtm":"2025-11-24T11:18:07Z","AppDtm":"2025-11-24T11:18:22Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:18:07Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.892112,"GPSLongitude":79.47622,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:18:07Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":30.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":90.7,"TDisQ":null,"FreqComp":null,"TSuc":-28.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":900,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":-0.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":407,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.62,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.28,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.101Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":23,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"82153526-fc19-4536-8dd4-846d36db6cb7","EventDtm":"2025-11-24T11:19:11Z","AppDtm":"2025-11-24T11:19:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:19:11Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.891919,"GPSLongitude":79.475917,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":32.3,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:19:11Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":31.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":74.9,"TDisQ":null,"FreqComp":null,"TSuc":-28.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":980,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":409.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":31.7,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.06,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.116Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":24,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ecd9db77-8f01-43d8-84a2-d443a4ee1e4d","EventDtm":"2025-11-24T11:19:15Z","AppDtm":"2025-11-24T11:19:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:19:15Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.516227,"GPSLongitude":82.962352,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"255596565","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":30.9,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:19:15Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":27.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":40,"PSucQ":"asProvided","TDis":86.8,"TDisQ":null,"FreqComp":null,"TSuc":-8.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":42,"PctExpVlvQ":null,"TEvap":21.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":390.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.7,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.37,"PctSucVlvQ":null,"TSup1":23,"TSup1Q":null,"TSup2":23,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.124Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":25,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b389932c-01b0-4604-9ff2-cd076eac1a6b","EventDtm":"2025-11-24T11:19:31Z","AppDtm":"2025-11-24T11:19:46Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:19:31Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":17.678669,"GPSLongitude":78.720211,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:19:31Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":28.69,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":20,"PSucQ":"asProvided","TDis":90.1,"TDisQ":null,"FreqComp":null,"TSuc":2.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":800,"PctExpVlvQ":"OOR","TEvap":2.69,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":83.86,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":401.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.69,"TRtn1Q":null,"TRtn2":5.6,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":14.33,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.139Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":26,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bf0dc768-ad30-4092-b612-a435394644e5","EventDtm":"2025-11-24T11:18:38Z","AppDtm":"2025-11-24T11:20:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:18:38Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.533221,"GPSLongitude":78.433059,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.4,"BatteryVoltage":8.1,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:18:38Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":30.12,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":64.7,"TDisQ":null,"FreqComp":null,"TSuc":17,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":960,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":14.96,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"off","FreqLine":50,"FreqLineQ":null,"VLine1":414.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.5,"TRtn1Q":null,"TRtn2":135.9,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":156.1,"PctSucVlvQ":null,"TSup1":4.62,"TSup1Q":null,"TSup2":4.6,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.151Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":27,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7fba5c07-3824-4d49-b3ba-2a475250769d","EventDtm":"2025-11-24T11:20:38Z","AppDtm":"2025-11-24T11:20:55Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:20:38Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":28.364714,"GPSLongitude":75.581333,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"255024908","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:20:38Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":22,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":36,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":6,"AmpPhB":6.9,"AmpPhC":6.8,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":400,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.4,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":6.5,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.160Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":28,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"433e6d31-999d-41b3-bc0b-fd22498d14b1","EventDtm":"2025-11-24T11:23:00Z","AppDtm":"2025-11-24T11:23:15Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:23:00Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804909,"GPSLongitude":77.662148,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:23:00Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.03,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":100.92,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.42,"AmpPhB":10.95,"AmpPhC":11.42,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.15,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.65,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.1,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.72,"TRtn1Q":null,"TRtn2":5.74,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.01,"PctSucVlvQ":null,"TSup1":4.9,"TSup1Q":null,"TSup2":4.83,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.165Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":29,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"29f27b34-8769-46c9-8e87-6ed24f229ba1","EventDtm":"2025-11-24T11:25:48Z","AppDtm":"2025-11-24T11:26:05Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:25:48Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":15.479483,"GPSLongitude":73.969705,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":28.9,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:25:48Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":30.97,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":155.65,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.48,"AmpPhB":9.88,"AmpPhC":10.48,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.04,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":89.64,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.82,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.69,"TRtn1Q":null,"TRtn2":5.7,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.86,"PctSucVlvQ":null,"TSup1":5.01,"TSup1Q":null,"TSup2":5.02,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.169Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":30,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"01952d8d-0097-4bf2-9b73-7a45b15336d8","EventDtm":"2025-11-24T11:26:07Z","AppDtm":"2025-11-24T11:26:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:26:07Z","DeviceID":"JSGA623040314","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":19.252876,"GPSLongitude":73.016548,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":28.8,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:26:07Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":31.34,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-189.06,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":145.41,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":10.11,"AmpPhB":10.82,"AmpPhC":10.11,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.92,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":390.53,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.06,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.42,"TRtn1Q":null,"TRtn2":5.53,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":4.93,"PctSucVlvQ":null,"TSup1":8.04,"TSup1Q":null,"TSup2":5.04,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.175Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":31,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5ee69656-a97e-4397-a85a-52a6d239895a","EventDtm":"2025-11-24T11:27:12Z","AppDtm":"2025-11-24T11:27:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:27:12Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.516108,"GPSLongitude":82.981215,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:27:12Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":28.13,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":125.73,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":12.03,"AmpPhB":11.04,"AmpPhC":12.03,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.17,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":95.52,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.68,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.01,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.63,"TRtn1Q":null,"TRtn2":3.67,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.24,"PctSucVlvQ":null,"TSup1":3,"TSup1Q":null,"TSup2":3.06,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.178Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":32,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"17a0f2ea-a2b7-4619-b0d0-a50f73ee3fce","EventDtm":"2025-11-24T11:30:50Z","AppDtm":"2025-11-24T11:31:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:30:50Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":16.89212,"GPSLongitude":79.476156,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-61","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:30:50Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":30.98,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-191.8,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":152.45,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":11.43,"AmpPhB":11.2,"AmpPhC":11.43,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.09,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.22,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":403.1,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.81,"TRtn1Q":null,"TRtn2":17.75,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.21,"PctSucVlvQ":null,"TSup1":18.51,"TSup1Q":null,"TSup2":18.54,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.179Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":33,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9d14b56e-a009-4f5d-ae29-3026f399828b","EventDtm":"2025-11-24T11:31:23Z","AppDtm":"2025-11-24T11:31:42Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:31:23Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.657881,"GPSLongitude":83.101659,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232723478","RSSI":"-81","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":7.9,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:31:23Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":27.83,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":70.72,"PSucQ":null,"TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":111.57,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.94,"AmpPhB":1.57,"AmpPhC":0.94,"PDis":129.84,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.28,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.01,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.98,"TRtn1Q":null,"TRtn2":21.01,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":20.1,"PctSucVlvQ":null,"TSup1":20.95,"TSup1Q":null,"TSup2":20.94,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.187Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":34,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1d4601bf-c696-4a16-81d0-a13bf039905f","EventDtm":"2025-11-24T11:31:45Z","AppDtm":"2025-11-24T11:32:07Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:31:45Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.80501,"GPSLongitude":77.6622,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:31:45Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":25.18,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":2,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":129.02,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":12.24,"AmpPhB":11.89,"AmpPhC":12.24,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":8.27,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.38,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.66,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.46,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":7.74,"TRtn1Q":null,"TRtn2":7.72,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":14.62,"PctSucVlvQ":null,"TSup1":5.77,"TSup1Q":null,"TSup2":5.81,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.192Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":35,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f2fef8bb-d19a-436a-96dc-acfce9ae3ec6","EventDtm":"2025-11-24T11:33:01Z","AppDtm":"2025-11-24T11:33:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:33:01Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804964,"GPSLongitude":77.662195,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:33:01Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.01,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":99.23,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.51,"AmpPhB":10.87,"AmpPhC":11.51,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.2,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.99,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.08,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.77,"TRtn1Q":null,"TRtn2":5.79,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.42,"PctSucVlvQ":null,"TSup1":5.08,"TSup1Q":null,"TSup2":5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.193Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":36,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c5c3f72f-80dd-4852-9c98-6d03a0a71b88","EventDtm":"2025-11-24T11:33:51Z","AppDtm":"2025-11-24T11:34:08Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:33:51Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.679068,"GPSLongitude":78.720214,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:33:51Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":28.05,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.42,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":155.01,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":10.99,"AmpPhB":10.54,"AmpPhC":10.99,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.49,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":99.16,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":408.75,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.12,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.54,"PctSucVlvQ":null,"TSup1":4.09,"TSup1Q":null,"TSup2":4.12,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.197Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":37,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0d6213fe-8f15-4dd6-bb4d-6de834a5f926","EventDtm":"2025-11-24T11:35:41Z","AppDtm":"2025-11-24T11:36:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:35:41Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":26.310544,"GPSLongitude":91.717649,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8.1,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:35:41Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":24,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":68.9,"TDisQ":null,"FreqComp":null,"TSuc":-28,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":850,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":72,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":395.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":85.06,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":10,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.198Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":38,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d7015d42-0a3d-4b1d-86c2-f3ee04497e0a","EventDtm":"2025-11-24T11:37:15Z","AppDtm":"2025-11-24T11:37:32Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:37:15Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.678745,"GPSLongitude":78.720237,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.3,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:37:15Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":27.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":220,"PSucQ":"asProvided","TDis":90.8,"TDisQ":null,"FreqComp":null,"TSuc":5.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":730,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":800,"PctExpVlvQ":"OOR","TEvap":3.19,"TEvapQ":null,"MCtrl3":"PTIEmergencyStop1","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":87.01,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":399.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":14.02,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":107,"RCAlias":"E107","RCSeverity":"Severe","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.199Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":39,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1af8a918-519e-4c2f-b597-964ea1668c97","EventDtm":"2025-11-24T11:40:49Z","AppDtm":"2025-11-24T11:41:03Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:40:49Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.678726,"GPSLongitude":78.720207,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:40:49Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":27.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":90,"PSucQ":"asProvided","TDis":52.3,"TDisQ":null,"FreqComp":null,"TSuc":13.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":900,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":400,"PctExpVlvQ":"OOR","TEvap":4.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":87.01,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":399.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":4.38,"TSup1Q":null,"TSup2":4.4,"TSup2Q":null,"AmpTotalDraw":1,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":40,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"40e7ab84-9bd1-48e9-a5b3-d3fb42c0c3f7","EventDtm":"2025-11-24T11:43:03Z","AppDtm":"2025-11-24T11:43:17Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:43:03Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.804974,"GPSLongitude":77.662125,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:43:03Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.11,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":109.79,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.45,"AmpPhB":11.09,"AmpPhC":11.45,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.8,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.02,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.78,"TRtn1Q":null,"TRtn2":5.8,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.58,"PctSucVlvQ":null,"TSup1":4.98,"TSup1Q":null,"TSup2":4.9,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.203Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":41,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0888fcdd-e470-4e64-b45a-0d4bf7c8a4ff","EventDtm":"2025-11-24T11:41:26Z","AppDtm":"2025-11-24T11:44:37Z","Events":["DeviceIsMoving"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:41:26Z","DeviceID":"JSGA622340507","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.703017,"GPSLongitude":83.156183,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"25623","CID":"233061644","RSSI":null,"ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.7,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6616969","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.205Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":42,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"20fa8081-65ff-42f8-a617-f27d4c285f3a","EventDtm":"2025-11-24T11:45:47Z","AppDtm":"2025-11-24T11:46:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:45:47Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.532998,"GPSLongitude":78.433267,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"230743318","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":32.8,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:45:47Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":28.69,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":73.5,"TDisQ":null,"FreqComp":null,"TSuc":-28.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":880,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":415.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.12,"TRtn1Q":null,"TRtn2":6.2,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.67,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.206Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":43,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8a0e8a3c-35a4-4bf1-88df-5b88be7bff2a","EventDtm":"2025-11-24T11:48:06Z","AppDtm":"2025-11-24T11:48:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:48:06Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657962,"GPSLongitude":83.10178,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8.1,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:48:06Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":28.4,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":71.51,"PSucQ":null,"TDis":-191.02,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":105.46,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.93,"AmpPhB":1.58,"AmpPhC":0.93,"PDis":105.34,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.03,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":428.63,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.87,"TRtn1Q":null,"TRtn2":20.94,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":19.68,"PctSucVlvQ":null,"TSup1":21.1,"TSup1Q":null,"TSup2":21.17,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.279Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":44,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"001c516c-f47d-4c80-a7d9-d088b5796cba","EventDtm":"2025-11-24T11:49:40Z","AppDtm":"2025-11-24T11:50:04Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:49:40Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":28.678683,"GPSLongitude":77.599725,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:49:40Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":23.7,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":54.21,"PSucQ":null,"TDis":70.51,"TDisQ":null,"FreqComp":null,"TSuc":16.59,"TSucQ":null,"MCond":0,"PCond":247.5,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04475864","AmpPhA":2.18,"AmpPhB":2.1,"AmpPhC":2.18,"PDis":107.96,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":17.06,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":70.34,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":49,"FreqLineQ":null,"VLine1":408.95,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":16.72,"TRtn1Q":null,"TRtn2":16.71,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":20,"PctSucVlvQ":null,"TSup1":16.53,"TSup1Q":null,"TSup2":16.58,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.280Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":45,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7734ae31-295b-4488-8e2f-fdb0c8153c2c","EventDtm":"2025-11-24T11:50:18Z","AppDtm":"2025-11-24T11:51:09Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:50:18Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":26.606072,"GPSLongitude":80.723734,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.281Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":46,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3492c7da-f78e-42cb-9bcf-31309b6f22f8","EventDtm":"2025-11-24T11:53:01Z","AppDtm":"2025-11-24T11:53:15Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:53:01Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.805008,"GPSLongitude":77.662159,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904096","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:53:01Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.4,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":100.3,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.48,"AmpPhB":10.78,"AmpPhC":11.48,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.14,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.04,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.05,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.71,"TRtn1Q":null,"TRtn2":5.73,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.52,"PctSucVlvQ":null,"TSup1":4.96,"TSup1Q":null,"TSup2":4.88,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":47,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"36016159-f32c-4079-ac5a-47caa06cd465","EventDtm":"2025-11-24T11:53:29Z","AppDtm":"2025-11-24T11:53:43Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:53:29Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.53902,"GPSLongitude":78.178275,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":32.1,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:53:29Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":28.88,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":109.9,"TDisQ":null,"FreqComp":null,"TSuc":-34.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":412.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":89.02,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.282Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":48,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"235da48e-e802-42d6-8953-663debd5148c","EventDtm":"2025-11-24T11:59:29Z","AppDtm":"2025-11-24T11:59:43Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:59:29Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":26.644482,"GPSLongitude":88.468073,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.2,"BatteryVoltage":8.1,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:59:29Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":22.69,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":59.1,"TDisQ":null,"FreqComp":null,"TSuc":-26.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":36,"PctExpVlvQ":null,"TEvap":-0.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":404.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":0.5,"TRtn1Q":null,"TRtn2":1.3,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":0,"TSup1Q":null,"TSup2":1.7,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.283Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":49,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"60e062ee-749a-4270-bdd0-ebe98ba91be7","EventDtm":"2025-11-24T11:59:55Z","AppDtm":"2025-11-24T12:00:12Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T11:59:55Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.824936,"GPSLongitude":78.131539,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T11:59:55Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":30.19,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":0,"PSucQ":"asProvided","TDis":72.8,"TDisQ":null,"FreqComp":null,"TSuc":-24.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1030,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":11.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":398.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.19,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":16,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":50,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"91b1a2c4-f283-4b42-8526-cd3330b8a432","EventDtm":"2025-11-24T12:01:20Z","AppDtm":"2025-11-24T12:01:40Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T12:01:20Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":21.735485,"GPSLongitude":72.628788,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":31.1,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T12:01:20Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":32.73,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":173.89,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":13.5,"AmpPhB":13.29,"AmpPhC":13.5,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.35,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":89,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":435.05,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.18,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.65,"TRtn1Q":null,"TRtn2":15.6,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.16,"PctSucVlvQ":null,"TSup1":15.19,"TSup1Q":null,"TSup2":15.37,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.286Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":51,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6bf829ed-64ac-4ecb-9aba-f59b4b46c675","EventDtm":"2025-11-24T12:02:09Z","AppDtm":"2025-11-24T12:02:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T12:02:09Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":15,"GPSLatitude":17.547924,"GPSLongitude":78.380646,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-55","ExtPower":true,"ExtPowerVoltage":33.3,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.299Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":52,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"78b4d23b-6c11-4caa-9f25-1422ff33e8f2","EventDtm":"2025-11-24T12:03:01Z","AppDtm":"2025-11-24T12:03:15Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T12:03:01Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":12.804878,"GPSLongitude":77.662161,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T12:03:01Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.76,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":97.17,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.54,"AmpPhB":11,"AmpPhC":11.54,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.22,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.1,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.79,"TRtn1Q":null,"TRtn2":5.81,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.92,"PctSucVlvQ":null,"TSup1":5.09,"TSup1Q":null,"TSup2":5.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.300Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":53,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"dc0fe504-e9a4-410e-adad-8c013cff69c6","EventDtm":"2025-11-24T12:05:04Z","AppDtm":"2025-11-24T12:05:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T12:05:04Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":2,"GPSLatitude":19.252975,"GPSLongitude":73.016419,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.302Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":54,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c8ccdc6e-b4f3-42fc-b710-eeaf6eef823f","EventDtm":"2025-11-24T13:51:14Z","AppDtm":"2025-11-24T12:09:56Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T13:51:14Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":2680,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":33.8,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":55,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4158d42a-12be-494c-a63d-494f1d5d3693","EventDtm":"2025-11-24T12:11:07Z","AppDtm":"2025-11-24T12:11:24Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T12:11:07Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.661588,"GPSLongitude":83.089131,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T12:11:07Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":30.5,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":110,"PSucQ":"asProvided","TDis":46.5,"TDisQ":null,"FreqComp":null,"TSuc":16,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1060,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":10,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":365.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":98.78,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:12:34.303Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":56,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2597b180-e04f-426e-a32f-10026a4f1a74","EventDtm":"2025-11-24T12:11:22Z","AppDtm":"2025-11-24T12:11:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T12:11:22Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.572256,"GPSLongitude":78.515017,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323414","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":33.3,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-24T12:36:32.777Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a9880985-0007-41ca-91da-8c9f77230694","EventDtm":"2025-11-24T12:35:43Z","AppDtm":"2025-11-24T12:35:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-24T12:35:43Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":26.310517,"GPSLongitude":91.717605,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":"-55","ExtPower":true,"ExtPowerVoltage":32.3,"BatteryVoltage":8.1,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-24T12:35:43Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":23,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":67.8,"TDisQ":null,"FreqComp":null,"TSuc":-27.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":72,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":402.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":84.45,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":10,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
   </si>
 </sst>
 </file>
@@ -504,7 +762,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -939,6 +1197,1446 @@
         <v>34</v>
       </c>
     </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" t="s">
+        <v>11</v>
+      </c>
+      <c r="J37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" t="s">
+        <v>11</v>
+      </c>
+      <c r="J41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+      <c r="J43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" t="s">
+        <v>11</v>
+      </c>
+      <c r="I44" t="s">
+        <v>11</v>
+      </c>
+      <c r="J44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" t="s">
+        <v>11</v>
+      </c>
+      <c r="J45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" t="s">
+        <v>11</v>
+      </c>
+      <c r="J49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>11</v>
+      </c>
+      <c r="I53" t="s">
+        <v>11</v>
+      </c>
+      <c r="J53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54" t="s">
+        <v>11</v>
+      </c>
+      <c r="J54" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" t="s">
+        <v>11</v>
+      </c>
+      <c r="I56" t="s">
+        <v>11</v>
+      </c>
+      <c r="J56" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" t="s">
+        <v>11</v>
+      </c>
+      <c r="J57" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" t="s">
+        <v>11</v>
+      </c>
+      <c r="I58" t="s">
+        <v>11</v>
+      </c>
+      <c r="J58" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>